<commit_message>
Update a source file and stopword list
</commit_message>
<xml_diff>
--- a/data/stopword_list.xlsx
+++ b/data/stopword_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gbpark/GBnotebook/mHealthapp-review-analysis1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EEC3A3-CD52-C548-B759-8220216F9B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FE5F95-E508-D54D-A1F4-40DE372A997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{FC117C88-87F2-F64E-BEB1-49D6CB2E0636}"/>
+    <workbookView xWindow="16860" yWindow="460" windowWidth="18980" windowHeight="21140" xr2:uid="{FC117C88-87F2-F64E-BEB1-49D6CB2E0636}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="940">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="959">
   <si>
     <t>stopword</t>
   </si>
@@ -2938,6 +2938,82 @@
   </si>
   <si>
     <t>예를 들자면</t>
+  </si>
+  <si>
+    <t>이것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>때문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건가요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이걸로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이닝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주세요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만큼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이번</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테크</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3350,10 +3426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBEFEF7-63E3-5643-97E0-D4F67F55F94C}">
-  <dimension ref="A1:A953"/>
+  <dimension ref="A1:A973"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A945" zoomScale="142" workbookViewId="0">
+      <selection activeCell="A974" sqref="A974"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -8126,6 +8202,106 @@
         <v>24</v>
       </c>
     </row>
+    <row r="954" spans="1:1">
+      <c r="A954" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="955" spans="1:1">
+      <c r="A955" s="1" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="956" spans="1:1">
+      <c r="A956" s="1" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="957" spans="1:1">
+      <c r="A957" s="1" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="958" spans="1:1">
+      <c r="A958" s="1" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="959" spans="1:1">
+      <c r="A959" s="1" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="960" spans="1:1">
+      <c r="A960" s="1" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="961" spans="1:1">
+      <c r="A961" s="1" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="962" spans="1:1">
+      <c r="A962" s="1" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="963" spans="1:1">
+      <c r="A963" s="1" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="964" spans="1:1">
+      <c r="A964" s="1" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="965" spans="1:1">
+      <c r="A965" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="966" spans="1:1">
+      <c r="A966" s="1" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="967" spans="1:1">
+      <c r="A967" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="968" spans="1:1">
+      <c r="A968" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="969" spans="1:1">
+      <c r="A969" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="970" spans="1:1">
+      <c r="A970" s="1" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="971" spans="1:1">
+      <c r="A971" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="972" spans="1:1">
+      <c r="A972" s="1" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="973" spans="1:1">
+      <c r="A973" s="1" t="s">
+        <v>958</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A1298">
     <sortCondition ref="A1260:A1298"/>

</xml_diff>